<commit_message>
various updates to support conversion
</commit_message>
<xml_diff>
--- a/CEI_to_TEI_CEI.xlsx
+++ b/CEI_to_TEI_CEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winslow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\CEI_TEIP5\tei_cei\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="733">
   <si>
     <t>front</t>
   </si>
@@ -2221,6 +2221,12 @@
   </si>
   <si>
     <t>biblScope</t>
+  </si>
+  <si>
+    <t>issued/quote/date</t>
+  </si>
+  <si>
+    <t>additions</t>
   </si>
 </sst>
 </file>
@@ -2579,8 +2585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3481,7 +3487,7 @@
         <v>585</v>
       </c>
       <c r="B82" t="s">
-        <v>28</v>
+        <v>732</v>
       </c>
       <c r="C82" s="6">
         <v>2</v>
@@ -3693,6 +3699,9 @@
     <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>605</v>
+      </c>
+      <c r="B102" t="s">
+        <v>731</v>
       </c>
       <c r="C102" s="6">
         <v>2</v>

</xml_diff>